<commit_message>
files updated/generated due to model runs
</commit_message>
<xml_diff>
--- a/models/calculation engines/economic_overlay/outputs/max_economic_tonnes/max_economic_tonnes.xlsx
+++ b/models/calculation engines/economic_overlay/outputs/max_economic_tonnes/max_economic_tonnes.xlsx
@@ -1272,10 +1272,10 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>6071.939999999991</v>
+        <v>6071.939999999992</v>
       </c>
       <c r="B105" t="n">
-        <v>4909.055062380726</v>
+        <v>6071.93999999999</v>
       </c>
     </row>
     <row r="106">
@@ -1312,18 +1312,18 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>922.0786875066219</v>
+        <v>1614.603374998454</v>
       </c>
       <c r="B110" t="n">
-        <v>353.1600000116985</v>
+        <v>773.6411249918334</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>4409.11875014827</v>
+        <v>5833.303125070232</v>
       </c>
       <c r="B111" t="n">
-        <v>2406.156250130062</v>
+        <v>3292.748958327263</v>
       </c>
     </row>
     <row r="112">
@@ -1339,7 +1339,7 @@
         <v>3026.099999999997</v>
       </c>
       <c r="B113" t="n">
-        <v>2022.803750004141</v>
+        <v>2789.685937499999</v>
       </c>
     </row>
     <row r="114">
@@ -1360,26 +1360,26 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>33595.06499999995</v>
+        <v>33595.06499999996</v>
       </c>
       <c r="B116" t="n">
-        <v>16642.55526581298</v>
+        <v>22691.66667199495</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>30296.54296862074</v>
+        <v>36194.27000000002</v>
       </c>
       <c r="B117" t="n">
-        <v>15129.42030204886</v>
+        <v>20429.29555182912</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>25298.28</v>
+        <v>25298.28000000001</v>
       </c>
       <c r="B118" t="n">
-        <v>24609.35362581317</v>
+        <v>25298.28000000001</v>
       </c>
     </row>
     <row r="119">
@@ -1416,58 +1416,58 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>18392.04832441613</v>
+        <v>23354.982</v>
       </c>
       <c r="B123" t="n">
-        <v>9289.861143829243</v>
+        <v>12341.30075618884</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>77939.01990000054</v>
+        <v>77939.01990000055</v>
       </c>
       <c r="B124" t="n">
-        <v>35918.05814368754</v>
+        <v>53493.7710538886</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>20995.24215633951</v>
+        <v>25055.59000000005</v>
       </c>
       <c r="B125" t="n">
-        <v>10712.01042718326</v>
+        <v>14720.15912496869</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>2609.180000000002</v>
+        <v>2609.180000000001</v>
       </c>
       <c r="B126" t="n">
-        <v>2159.562374990678</v>
+        <v>2609.179999999996</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>3210.199999999995</v>
+        <v>3210.199999999996</v>
       </c>
       <c r="B127" t="n">
-        <v>2296.343958337724</v>
+        <v>3094.116875034388</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>32620.16897054895</v>
+        <v>41643.55999999989</v>
       </c>
       <c r="B128" t="n">
-        <v>16337.0412545343</v>
+        <v>22413.77859607097</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>4780.719239640359</v>
+        <v>5770.870000000005</v>
       </c>
       <c r="B129" t="n">
-        <v>2271.421302047609</v>
+        <v>3773.393270846046</v>
       </c>
     </row>
     <row r="130">
@@ -1480,10 +1480,10 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>6439.600000059198</v>
+        <v>6629.000000000012</v>
       </c>
       <c r="B131" t="n">
-        <v>3403.281250039062</v>
+        <v>5067.436458377922</v>
       </c>
     </row>
     <row r="132">
@@ -1496,34 +1496,34 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>88831.96000000015</v>
+        <v>88831.96000000014</v>
       </c>
       <c r="B133" t="n">
-        <v>74277.79512404837</v>
+        <v>88831.96000000022</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>4373.040000033836</v>
+        <v>6344.099999942547</v>
       </c>
       <c r="B134" t="n">
-        <v>2002.979999976379</v>
+        <v>3270.204000019151</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>20939.66718758787</v>
+        <v>27864.26999999993</v>
       </c>
       <c r="B135" t="n">
-        <v>10374.4648125995</v>
+        <v>14873.38340636111</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>33580.81650021808</v>
+        <v>47456.25228657518</v>
       </c>
       <c r="B136" t="n">
-        <v>15836.05488719246</v>
+        <v>21519.53276031595</v>
       </c>
     </row>
     <row r="137">

</xml_diff>